<commit_message>
Added new test data.
</commit_message>
<xml_diff>
--- a/data/orders.xlsx
+++ b/data/orders.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{205F076B-8C31-4156-A153-B0DBF0E4816E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2DC6ADFF-AE6F-4F28-8DE3-D4FE7D0BF7D1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="906" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="906" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin payment types" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,16 @@
     <sheet name="Customer valid discounts" sheetId="8" r:id="rId8"/>
     <sheet name="Customer invalid discounts" sheetId="10" r:id="rId9"/>
     <sheet name="Admin certificates" sheetId="11" r:id="rId10"/>
+    <sheet name="Admin certificates declines" sheetId="12" r:id="rId11"/>
+    <sheet name="Customer certificates" sheetId="13" r:id="rId12"/>
+    <sheet name="Customer certificates declines" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3065" uniqueCount="956">
   <si>
     <t>id_testdata</t>
   </si>
@@ -2448,13 +2451,457 @@
   </si>
   <si>
     <t>38.86</t>
+  </si>
+  <si>
+    <t>GoDo-743</t>
+  </si>
+  <si>
+    <t>Thornton</t>
+  </si>
+  <si>
+    <t>GoDo-744</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>GoDo-745</t>
+  </si>
+  <si>
+    <t>Joann</t>
+  </si>
+  <si>
+    <t>Nguyen</t>
+  </si>
+  <si>
+    <t>GoDo-746</t>
+  </si>
+  <si>
+    <t>Garry</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>GoDo-747</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Cross</t>
+  </si>
+  <si>
+    <t>GoDo-748</t>
+  </si>
+  <si>
+    <t>Joey</t>
+  </si>
+  <si>
+    <t>Kelley</t>
+  </si>
+  <si>
+    <t>GoDo-749</t>
+  </si>
+  <si>
+    <t>Darla</t>
+  </si>
+  <si>
+    <t>Townsend</t>
+  </si>
+  <si>
+    <t>GoDo-750</t>
+  </si>
+  <si>
+    <t>Dawn</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>GoDo-751</t>
+  </si>
+  <si>
+    <t>Norman</t>
+  </si>
+  <si>
+    <t>Byrd</t>
+  </si>
+  <si>
+    <t>GoDo-752</t>
+  </si>
+  <si>
+    <t>Kayla</t>
+  </si>
+  <si>
+    <t>Walsh</t>
+  </si>
+  <si>
+    <t>godo-743ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-744ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-745ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-746ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-747ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-748ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-749ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-750ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-751ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-752ac@mailinator.com</t>
+  </si>
+  <si>
+    <t>GoDo-46</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>60.00</t>
+  </si>
+  <si>
+    <t>1060.00</t>
+  </si>
+  <si>
+    <t>GoDo-47</t>
+  </si>
+  <si>
+    <t>de Medici</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>30.00</t>
+  </si>
+  <si>
+    <t>530.00</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>53.00</t>
+  </si>
+  <si>
+    <t>Marry-Key</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>Wong</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>URL_cert</t>
+  </si>
+  <si>
+    <t>godo-46ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-47ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-473ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-474ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-475ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-476ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-477ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-478ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-am_ex-ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-479ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-discover-ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-480-ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-diners_club-ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-481-ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-unionpay-ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-482ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-483ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-484ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>https://dev.godo.io/customerGiftCertificate.aspx?company_guid=b7308a3a-448a-48f1-838f-c2d21d2c6037</t>
+  </si>
+  <si>
+    <t>Ghosts &amp; Spirits Walking Tour</t>
+  </si>
+  <si>
+    <t>Gray Line New Orleans - Walking Tour</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>94.34</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>9.48</t>
+  </si>
+  <si>
+    <t>167.48</t>
+  </si>
+  <si>
+    <t>26.50</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>68.90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adults (12+) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children (6-12) </t>
+  </si>
+  <si>
+    <t>42.38</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>1.62</t>
+  </si>
+  <si>
+    <t>28.62</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>79.50</t>
+  </si>
+  <si>
+    <t>4.50</t>
+  </si>
+  <si>
+    <t>238.50</t>
+  </si>
+  <si>
+    <t>13.50</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>Group (min of 10 adults)</t>
+  </si>
+  <si>
+    <t>242.5</t>
+  </si>
+  <si>
+    <t>14.55</t>
+  </si>
+  <si>
+    <t>257.05</t>
+  </si>
+  <si>
+    <t>52.98</t>
+  </si>
+  <si>
+    <t>15.90</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>GoDo-712</t>
+  </si>
+  <si>
+    <t>Emmett</t>
+  </si>
+  <si>
+    <t>Woods</t>
+  </si>
+  <si>
+    <t>GoDo-713</t>
+  </si>
+  <si>
+    <t>Antonia</t>
+  </si>
+  <si>
+    <t>Figueroa</t>
+  </si>
+  <si>
+    <t>GoDo-714</t>
+  </si>
+  <si>
+    <t>Terrell</t>
+  </si>
+  <si>
+    <t>Schmidt</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>106.00</t>
+  </si>
+  <si>
+    <t>GoDo-715</t>
+  </si>
+  <si>
+    <t>Latoya</t>
+  </si>
+  <si>
+    <t>Morrison</t>
+  </si>
+  <si>
+    <t>GoDo-716</t>
+  </si>
+  <si>
+    <t>Marshall</t>
+  </si>
+  <si>
+    <t>Bush</t>
+  </si>
+  <si>
+    <t>GoDo-717</t>
+  </si>
+  <si>
+    <t>Doug</t>
+  </si>
+  <si>
+    <t>Stewart</t>
+  </si>
+  <si>
+    <t>GoDo-718</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>GoDo-719</t>
+  </si>
+  <si>
+    <t>Perry</t>
+  </si>
+  <si>
+    <t>Lindsey</t>
+  </si>
+  <si>
+    <t>GoDo-720</t>
+  </si>
+  <si>
+    <t>Alison</t>
+  </si>
+  <si>
+    <t>Mccarthy</t>
+  </si>
+  <si>
+    <t>GoDo-721</t>
+  </si>
+  <si>
+    <t>Laurie</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>godo-712ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-713ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-714ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-715ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-716ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-717ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-718ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-719ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-720ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-721ic@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2474,6 +2921,21 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -2518,7 +2980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2537,6 +2999,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4315,9 +4782,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AB0DF-12AC-414D-A33D-AB09F26711FA}">
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L24" sqref="L24"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5301,6 +5768,2209 @@
       <c r="V25" s="1" t="s">
         <v>117</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B17890C-C3E9-4501-8241-BF8928D0B274}">
+  <dimension ref="A1:V25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S1" sqref="S1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="23.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="31.140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="31" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="28.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11" style="1" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="15" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="15" style="1" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="E2" t="s">
+        <v>837</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="1">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="E3" t="s">
+        <v>838</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="E4" t="s">
+        <v>839</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E5" t="s">
+        <v>840</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="E6" t="s">
+        <v>841</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="E7" t="s">
+        <v>842</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E8" t="s">
+        <v>843</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="E9" t="s">
+        <v>844</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="E10" t="s">
+        <v>845</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" s="1">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="E11" t="s">
+        <v>846</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E13"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E15"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E16"/>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E17"/>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E18"/>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E19"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC4B839-C73B-41C2-80DD-208DE6D431F6}">
+  <dimension ref="A1:U25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G14" sqref="G14:Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="39.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="31.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="31" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="18.5703125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="11" style="1" customWidth="1"/>
+    <col min="28" max="28" width="14.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5703125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15" style="1" customWidth="1"/>
+    <col min="32" max="32" width="13.7109375" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15" style="1" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="B2" t="s">
+        <v>883</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="F2" t="s">
+        <v>865</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>854</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>866</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>626</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>627</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>867</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" s="5">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>868</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>855</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>869</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>888</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>889</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>870</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>871</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>872</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>897</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>896</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>873</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>859</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>874</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U11" s="5">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>875</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U12" s="5">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>721</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>876</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>855</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>877</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>898</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>878</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>879</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>880</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>881</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>859</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>862</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>863</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>882</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>907</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDAFE5F-B530-4B77-9E58-E2B81982123D}">
+  <dimension ref="A1:V25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="39.7109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="5" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="31.140625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="31" style="5" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" style="5" customWidth="1"/>
+    <col min="19" max="19" width="28.5703125" style="5" customWidth="1"/>
+    <col min="20" max="20" width="16" style="5" customWidth="1"/>
+    <col min="21" max="21" width="15" style="5" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" style="5" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="5" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" style="5" customWidth="1"/>
+    <col min="25" max="25" width="20" style="5" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="5" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="5" customWidth="1"/>
+    <col min="28" max="28" width="11" style="5" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" style="5" customWidth="1"/>
+    <col min="30" max="30" width="13.28515625" style="5" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" style="5" customWidth="1"/>
+    <col min="32" max="32" width="15" style="5" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="5" customWidth="1"/>
+    <col min="34" max="34" width="15" style="5" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" style="5" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>864</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>604</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>914</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>916</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>946</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="5">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>918</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>947</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>855</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>948</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>926</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>928</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>949</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>929</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>930</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>950</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>855</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>951</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>855</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>936</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>952</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>898</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>937</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>938</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>939</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>953</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>940</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>941</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>954</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" s="5">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>943</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>944</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>955</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="D19" s="17"/>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="15"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10057,7 +12727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5157F94-0C19-4E79-93C8-C8C1FAC3D8AF}">
   <dimension ref="A1:AE13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -11090,7 +13760,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y17" sqref="Y17"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added test for purchasing gift certificates via call center.
</commit_message>
<xml_diff>
--- a/data/orders.xlsx
+++ b/data/orders.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2DC6ADFF-AE6F-4F28-8DE3-D4FE7D0BF7D1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5F57B1AD-03DE-40A1-883E-10955CC4D81B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="906" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="906" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin payment types" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,17 @@
     <sheet name="Admin certificates declines" sheetId="12" r:id="rId11"/>
     <sheet name="Customer certificates" sheetId="13" r:id="rId12"/>
     <sheet name="Customer certificates declines" sheetId="14" r:id="rId13"/>
+    <sheet name="Center payment types" sheetId="15" r:id="rId14"/>
+    <sheet name="Center declines" sheetId="16" r:id="rId15"/>
+    <sheet name="Center certificates" sheetId="17" r:id="rId16"/>
+    <sheet name="Center certificates declines" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3065" uniqueCount="956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3941" uniqueCount="1098">
   <si>
     <t>id_testdata</t>
   </si>
@@ -2895,6 +2899,432 @@
   </si>
   <si>
     <t>godo-721ic@mailinator.com</t>
+  </si>
+  <si>
+    <t>GoDo-315cb</t>
+  </si>
+  <si>
+    <t>GoDo-Cash -cb</t>
+  </si>
+  <si>
+    <t>GoDo-473cb</t>
+  </si>
+  <si>
+    <t>GoDo-474cb</t>
+  </si>
+  <si>
+    <t>GoDo-475cb</t>
+  </si>
+  <si>
+    <t>GoDo-476cb</t>
+  </si>
+  <si>
+    <t>GoDo-477cb</t>
+  </si>
+  <si>
+    <t>GoDo-478cb</t>
+  </si>
+  <si>
+    <t>GoDo-Am Express-cb</t>
+  </si>
+  <si>
+    <t>GoDo-479cb</t>
+  </si>
+  <si>
+    <t>GoDo-Discover-cb</t>
+  </si>
+  <si>
+    <t>GoDo-480cb</t>
+  </si>
+  <si>
+    <t>GoDo-Diners Club-cb</t>
+  </si>
+  <si>
+    <t>GoDo-481cb</t>
+  </si>
+  <si>
+    <t>GoDo-UnionPay-cb</t>
+  </si>
+  <si>
+    <t>GoDo-482cb</t>
+  </si>
+  <si>
+    <t>GoDo-483cb</t>
+  </si>
+  <si>
+    <t>GoDo-484cb</t>
+  </si>
+  <si>
+    <t>godo-315cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-cash-cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-473cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-474cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-475cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-476cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-477cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-478cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-am_ex_cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-479cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-discover_cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-480cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-diners_club_cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-481cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-unionpay_cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-482cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-483cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-484cb@mailinator.com</t>
+  </si>
+  <si>
+    <t>9:30 PM CT</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>Olson</t>
+  </si>
+  <si>
+    <t>Howell</t>
+  </si>
+  <si>
+    <t>Sylvester</t>
+  </si>
+  <si>
+    <t>Suzanne</t>
+  </si>
+  <si>
+    <t>Tabitha</t>
+  </si>
+  <si>
+    <t>Tate</t>
+  </si>
+  <si>
+    <t>Percy</t>
+  </si>
+  <si>
+    <t>Richards</t>
+  </si>
+  <si>
+    <t>Hope</t>
+  </si>
+  <si>
+    <t>Newman</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Kennedy</t>
+  </si>
+  <si>
+    <t>Stuart</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Sherman</t>
+  </si>
+  <si>
+    <t>Sheldon</t>
+  </si>
+  <si>
+    <t>Sharp</t>
+  </si>
+  <si>
+    <t>Vivian</t>
+  </si>
+  <si>
+    <t>Mann</t>
+  </si>
+  <si>
+    <t>Cathy</t>
+  </si>
+  <si>
+    <t>Reyes</t>
+  </si>
+  <si>
+    <t>Parsons</t>
+  </si>
+  <si>
+    <t>Abel</t>
+  </si>
+  <si>
+    <t>Melba</t>
+  </si>
+  <si>
+    <t>Sullivan</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
+    <t>Lambert</t>
+  </si>
+  <si>
+    <t>Luther</t>
+  </si>
+  <si>
+    <t>Maxwell</t>
+  </si>
+  <si>
+    <t>$6.34</t>
+  </si>
+  <si>
+    <t>$5.14</t>
+  </si>
+  <si>
+    <t>$12.68</t>
+  </si>
+  <si>
+    <t>$10.28</t>
+  </si>
+  <si>
+    <t>$99.79</t>
+  </si>
+  <si>
+    <t>$77.59</t>
+  </si>
+  <si>
+    <t>$155.18</t>
+  </si>
+  <si>
+    <t>$199.58</t>
+  </si>
+  <si>
+    <t>GoDo-644</t>
+  </si>
+  <si>
+    <t>godo-644cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>35.00</t>
+  </si>
+  <si>
+    <t>Tommy</t>
+  </si>
+  <si>
+    <t>Reeves</t>
+  </si>
+  <si>
+    <t>Mills</t>
+  </si>
+  <si>
+    <t>Thelma</t>
+  </si>
+  <si>
+    <t>Clarke</t>
+  </si>
+  <si>
+    <t>Welch</t>
+  </si>
+  <si>
+    <t>Allan</t>
+  </si>
+  <si>
+    <t>Banks</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Blair</t>
+  </si>
+  <si>
+    <t>Maxine</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>GoDo-645</t>
+  </si>
+  <si>
+    <t>GoDo-646</t>
+  </si>
+  <si>
+    <t>GoDo-647</t>
+  </si>
+  <si>
+    <t>GoDo-649</t>
+  </si>
+  <si>
+    <t>GoDo-651</t>
+  </si>
+  <si>
+    <t>GoDo-652</t>
+  </si>
+  <si>
+    <t>GoDo-653</t>
+  </si>
+  <si>
+    <t>godo-645cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-646cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-647cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-649cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-651cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-652cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-653cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>90.00</t>
+  </si>
+  <si>
+    <t>GoDo-743-cc</t>
+  </si>
+  <si>
+    <t>GoDo-744-cc</t>
+  </si>
+  <si>
+    <t>GoDo-745-cc</t>
+  </si>
+  <si>
+    <t>GoDo-746-cc</t>
+  </si>
+  <si>
+    <t>GoDo-747-cc</t>
+  </si>
+  <si>
+    <t>GoDo-748-cc</t>
+  </si>
+  <si>
+    <t>GoDo-749-cc</t>
+  </si>
+  <si>
+    <t>GoDo-750-cc</t>
+  </si>
+  <si>
+    <t>GoDo-751-cc</t>
+  </si>
+  <si>
+    <t>GoDo-752-cc</t>
+  </si>
+  <si>
+    <t>godo-743cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-744cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-745cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-746cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-747cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-748cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-749cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-750cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-751cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>godo-752cc@mailinator.com</t>
+  </si>
+  <si>
+    <t>Teresa</t>
+  </si>
+  <si>
+    <t>Crawford</t>
+  </si>
+  <si>
+    <t>Nichole</t>
+  </si>
+  <si>
+    <t>Ida</t>
+  </si>
+  <si>
+    <t>Guzman</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t>Fuller</t>
+  </si>
+  <si>
+    <t>Roxanne</t>
+  </si>
+  <si>
+    <t>Mclaughlin</t>
+  </si>
+  <si>
+    <t>Mandy</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
+    <t>Freda</t>
+  </si>
+  <si>
+    <t>Stacy</t>
+  </si>
+  <si>
+    <t>Lamar</t>
+  </si>
+  <si>
+    <t>Garcia</t>
   </si>
 </sst>
 </file>
@@ -7332,9 +7762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDAFE5F-B530-4B77-9E58-E2B81982123D}">
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7971,6 +8401,3356 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F25" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C151C05-E2F4-455A-AEB9-6524417D8442}">
+  <dimension ref="A1:AA40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Y24" sqref="Y24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="38.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="15" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="15" style="1" customWidth="1"/>
+    <col min="27" max="27" width="15.42578125" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="N2" t="s">
+        <v>974</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="N3" t="s">
+        <v>975</v>
+      </c>
+      <c r="O3" s="1">
+        <v>35801</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="N4" t="s">
+        <v>976</v>
+      </c>
+      <c r="O4" s="1">
+        <v>35801</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="1">
+        <v>35801</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="N6" t="s">
+        <v>978</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N7" t="s">
+        <v>979</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="N8" t="s">
+        <v>980</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="N9" t="s">
+        <v>981</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="N10" t="s">
+        <v>982</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="N11" t="s">
+        <v>983</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T11" s="1">
+        <v>35801</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="N12" t="s">
+        <v>984</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" s="1">
+        <v>35801</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="N13" t="s">
+        <v>985</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="N14" t="s">
+        <v>986</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="N15" t="s">
+        <v>987</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N16" t="s">
+        <v>988</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N17" t="s">
+        <v>989</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="N18" t="s">
+        <v>990</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="N19" t="s">
+        <v>991</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="N21"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="N23"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="N24"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="N25"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="N26"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="N27"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="N28"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="N29"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="N30"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="N31"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="N32"/>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="N33"/>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="N34"/>
+    </row>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="N35"/>
+    </row>
+    <row r="36" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="N36"/>
+    </row>
+    <row r="37" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="N37"/>
+    </row>
+    <row r="38" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C91F198-B38A-4DA8-A78C-ABC8E5EDC3C9}">
+  <dimension ref="A1:AE17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="38.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="23.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="22.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5703125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="15" style="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="15" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="18" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R2" t="s">
+        <v>464</v>
+      </c>
+      <c r="S2" s="1">
+        <v>35801</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>35801</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R3" t="s">
+        <v>465</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R4" t="s">
+        <v>466</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R5" t="s">
+        <v>467</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R6" t="s">
+        <v>468</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R7" t="s">
+        <v>469</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R8" t="s">
+        <v>470</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R9" t="s">
+        <v>471</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R10" t="s">
+        <v>471</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>35801</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R11" t="s">
+        <v>472</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R12"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R13"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R14"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R15"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R16"/>
+    </row>
+    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8AF431-8396-45B8-B7F5-A36FBD82D208}">
+  <dimension ref="A1:V36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="23.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="31.140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="31" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="21.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11" style="1" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="15" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="15" style="1" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1058</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E10"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E11"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E13"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E14"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E15"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E16"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E17"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D18" s="13"/>
+      <c r="E18"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E19"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E20"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E21"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E22"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E23"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E24"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E25"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E26"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E27"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E28"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E29"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E30"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E31"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E32"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E33"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E34"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+    </row>
+    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+    </row>
+    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147B5EB0-EC16-485B-8EB9-BF6E6861C707}">
+  <dimension ref="A1:V25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="23.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="31.140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="31" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="28.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11" style="1" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="15" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="15" style="1" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="1">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" s="1">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E13"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E15"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E16"/>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E17"/>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E18"/>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E19"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13757,10 +17537,10 @@
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13931,6 +17711,9 @@
       <c r="AA2" s="1" t="s">
         <v>668</v>
       </c>
+      <c r="AB2" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="AC2" s="1" t="s">
         <v>165</v>
       </c>
@@ -13981,6 +17764,9 @@
       <c r="AA3" s="1" t="s">
         <v>668</v>
       </c>
+      <c r="AB3" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="AC3" s="1" t="s">
         <v>165</v>
       </c>
@@ -14031,6 +17817,9 @@
       <c r="AA4" s="1" t="s">
         <v>700</v>
       </c>
+      <c r="AB4" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="AC4" s="1" t="s">
         <v>701</v>
       </c>
@@ -14087,6 +17876,9 @@
       <c r="AA5" s="1" t="s">
         <v>661</v>
       </c>
+      <c r="AB5" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="AC5" s="1" t="s">
         <v>565</v>
       </c>
@@ -14137,6 +17929,9 @@
       <c r="AA6" s="1" t="s">
         <v>700</v>
       </c>
+      <c r="AB6" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="AC6" s="1" t="s">
         <v>701</v>
       </c>
@@ -14193,6 +17988,9 @@
       <c r="AA7" s="1" t="s">
         <v>711</v>
       </c>
+      <c r="AB7" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="AC7" s="1" t="s">
         <v>563</v>
       </c>
@@ -14249,6 +18047,9 @@
       <c r="AA8" s="1" t="s">
         <v>706</v>
       </c>
+      <c r="AB8" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="AC8" s="1" t="s">
         <v>708</v>
       </c>
@@ -14298,6 +18099,9 @@
       </c>
       <c r="AA9" s="1" t="s">
         <v>700</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="AC9" s="1" t="s">
         <v>701</v>

</xml_diff>

<commit_message>
Added tests for Add-ons.
</commit_message>
<xml_diff>
--- a/data/orders.xlsx
+++ b/data/orders.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D6128950-C443-4953-8DAA-967E862F6045}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4FD1FE6A-A9FD-4897-A6A5-5A7EBF42261F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="913" firstSheet="14" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="913" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin payment types" sheetId="1" r:id="rId1"/>
@@ -16,31 +16,32 @@
     <sheet name="Admin booking with certificates" sheetId="9" r:id="rId6"/>
     <sheet name="Admin cert + discount" sheetId="19" r:id="rId7"/>
     <sheet name="Admin groupon" sheetId="26" r:id="rId8"/>
-    <sheet name="Admin certificates" sheetId="11" r:id="rId9"/>
-    <sheet name="Admin certificates declines" sheetId="12" r:id="rId10"/>
-    <sheet name="Customer payment types" sheetId="4" r:id="rId11"/>
-    <sheet name="Customer declines" sheetId="5" r:id="rId12"/>
-    <sheet name="Customer not finished" sheetId="23" r:id="rId13"/>
-    <sheet name="Customer valid discounts" sheetId="8" r:id="rId14"/>
-    <sheet name="Customer invalid discounts" sheetId="10" r:id="rId15"/>
-    <sheet name="Customer certificates" sheetId="13" r:id="rId16"/>
-    <sheet name="Customer certificates declines" sheetId="14" r:id="rId17"/>
-    <sheet name="Customer booking with cert" sheetId="20" r:id="rId18"/>
-    <sheet name="Customer booking cert + disc" sheetId="25" r:id="rId19"/>
-    <sheet name="Customer groupon" sheetId="27" r:id="rId20"/>
-    <sheet name="Center payment types" sheetId="15" r:id="rId21"/>
-    <sheet name="Center declines" sheetId="16" r:id="rId22"/>
-    <sheet name="Center certificates" sheetId="17" r:id="rId23"/>
-    <sheet name="Center certificates declines" sheetId="18" r:id="rId24"/>
-    <sheet name="Failed declines" sheetId="21" r:id="rId25"/>
-    <sheet name="Emails table" sheetId="24" r:id="rId26"/>
+    <sheet name="Addons" sheetId="28" r:id="rId9"/>
+    <sheet name="Admin certificates" sheetId="11" r:id="rId10"/>
+    <sheet name="Admin certificates declines" sheetId="12" r:id="rId11"/>
+    <sheet name="Customer payment types" sheetId="4" r:id="rId12"/>
+    <sheet name="Customer declines" sheetId="5" r:id="rId13"/>
+    <sheet name="Customer not finished" sheetId="23" r:id="rId14"/>
+    <sheet name="Customer valid discounts" sheetId="8" r:id="rId15"/>
+    <sheet name="Customer invalid discounts" sheetId="10" r:id="rId16"/>
+    <sheet name="Customer certificates" sheetId="13" r:id="rId17"/>
+    <sheet name="Customer certificates declines" sheetId="14" r:id="rId18"/>
+    <sheet name="Customer booking with cert" sheetId="20" r:id="rId19"/>
+    <sheet name="Customer booking cert + disc" sheetId="25" r:id="rId20"/>
+    <sheet name="Customer groupon" sheetId="27" r:id="rId21"/>
+    <sheet name="Center payment types" sheetId="15" r:id="rId22"/>
+    <sheet name="Center declines" sheetId="16" r:id="rId23"/>
+    <sheet name="Center certificates" sheetId="17" r:id="rId24"/>
+    <sheet name="Center certificates declines" sheetId="18" r:id="rId25"/>
+    <sheet name="Failed declines" sheetId="21" r:id="rId26"/>
+    <sheet name="Emails table" sheetId="24" r:id="rId27"/>
   </sheets>
   <calcPr calcId="122211" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6751" uniqueCount="1541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6818" uniqueCount="1556">
   <si>
     <t>id_testdata</t>
   </si>
@@ -4663,6 +4664,51 @@
   </si>
   <si>
     <t>godo-842ib@mailinator.com</t>
+  </si>
+  <si>
+    <t>addon_name</t>
+  </si>
+  <si>
+    <t>addon_type</t>
+  </si>
+  <si>
+    <t>GoDo-206</t>
+  </si>
+  <si>
+    <t>Rosemary</t>
+  </si>
+  <si>
+    <t>godo-206ab@mailinator.com</t>
+  </si>
+  <si>
+    <t>New type, $10.99</t>
+  </si>
+  <si>
+    <t>addon</t>
+  </si>
+  <si>
+    <t>$10.99</t>
+  </si>
+  <si>
+    <t>$5.00</t>
+  </si>
+  <si>
+    <t>$104.99</t>
+  </si>
+  <si>
+    <t>Barker</t>
+  </si>
+  <si>
+    <t>GoDo-207</t>
+  </si>
+  <si>
+    <t>GoDo-221</t>
+  </si>
+  <si>
+    <t>GoDo-236</t>
+  </si>
+  <si>
+    <t>Inactive type, $50</t>
   </si>
 </sst>
 </file>
@@ -6562,6 +6608,1003 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AB0DF-12AC-414D-A33D-AB09F26711FA}">
+  <dimension ref="A1:V25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="23.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="31.140625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="31" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="21.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="20" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11" style="1" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="13.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5703125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="15" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="15" style="1" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" style="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="E2" t="s">
+        <v>787</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="E3" t="s">
+        <v>788</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="E4" t="s">
+        <v>789</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="E5" t="s">
+        <v>790</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>804</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="E6" t="s">
+        <v>791</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="E7" t="s">
+        <v>792</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="E8" t="s">
+        <v>793</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="E9" t="s">
+        <v>794</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="E10" t="s">
+        <v>742</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" s="1">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="E11" t="s">
+        <v>745</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="E12" t="s">
+        <v>748</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="E13" t="s">
+        <v>751</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="E14" t="s">
+        <v>754</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E15" t="s">
+        <v>756</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="E16" t="s">
+        <v>760</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="E17" t="s">
+        <v>763</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V17" s="1">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="E18" t="s">
+        <v>766</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V18" s="1">
+        <v>35801</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="E19" t="s">
+        <v>769</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>804</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="E20" t="s">
+        <v>772</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E21" t="s">
+        <v>774</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="E22" t="s">
+        <v>777</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="E23" t="s">
+        <v>780</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="E24" t="s">
+        <v>783</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="E25" t="s">
+        <v>786</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B17890C-C3E9-4501-8241-BF8928D0B274}">
   <dimension ref="A1:V23"/>
   <sheetViews>
@@ -7056,7 +8099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB17"/>
   <sheetViews>
@@ -8236,7 +9279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA15"/>
   <sheetViews>
@@ -8932,7 +9975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D291D8-D7EB-4761-A388-783D2E185CA1}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
@@ -9600,7 +10643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5157F94-0C19-4E79-93C8-C8C1FAC3D8AF}">
   <dimension ref="A1:AE13"/>
   <sheetViews>
@@ -10629,7 +11672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477A7A26-CD8B-4B4F-912F-0FE24C8401B2}">
   <dimension ref="A1:AE9"/>
   <sheetViews>
@@ -11216,7 +12259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC4B839-C73B-41C2-80DD-208DE6D431F6}">
   <dimension ref="A1:U25"/>
   <sheetViews>
@@ -12198,11 +13241,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDAFE5F-B530-4B77-9E58-E2B81982123D}">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
     </sheetView>
@@ -12760,7 +13803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D5B620-B0D6-437E-AF7B-E893E6927C23}">
   <dimension ref="A1:BB10"/>
   <sheetViews>
@@ -13954,7 +14997,734 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AE15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R2" sqref="R2:R9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="38.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="23.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="22.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5703125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="15" style="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="15" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="18" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R2" t="s">
+        <v>464</v>
+      </c>
+      <c r="S2" s="1">
+        <v>35801</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>35801</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R3" t="s">
+        <v>465</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R4" t="s">
+        <v>466</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R5" t="s">
+        <v>467</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R6" t="s">
+        <v>468</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R7" t="s">
+        <v>471</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R8" t="s">
+        <v>471</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>35801</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="R9" t="s">
+        <v>472</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R10"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R11"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R12"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R13"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R14"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="R15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66885A8D-1970-49DC-A0CB-66F933E2B20D}">
   <dimension ref="A1:BC17"/>
   <sheetViews>
@@ -15973,734 +17743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AE15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R2" sqref="R2:R9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="38.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="23.7109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="22.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="12.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="11" style="1" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="10.5703125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="15" style="1" customWidth="1"/>
-    <col min="29" max="29" width="13.7109375" style="1" customWidth="1"/>
-    <col min="30" max="30" width="15" style="1" customWidth="1"/>
-    <col min="31" max="31" width="15.42578125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="18" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>15044466025</v>
-      </c>
-      <c r="R2" t="s">
-        <v>464</v>
-      </c>
-      <c r="S2" s="1">
-        <v>35801</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>35801</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>15044466025</v>
-      </c>
-      <c r="R3" t="s">
-        <v>465</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>15044466025</v>
-      </c>
-      <c r="R4" t="s">
-        <v>466</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>15044466025</v>
-      </c>
-      <c r="R5" t="s">
-        <v>467</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>15044466025</v>
-      </c>
-      <c r="R6" t="s">
-        <v>468</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE6" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>15044466025</v>
-      </c>
-      <c r="R7" t="s">
-        <v>471</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE7" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>15044466025</v>
-      </c>
-      <c r="R8" t="s">
-        <v>471</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>35801</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE8" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>15044466025</v>
-      </c>
-      <c r="R9" t="s">
-        <v>472</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R10"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R11"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R12"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R13"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R14"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C4359E-4B78-467E-B2B7-C2E3C34B28DE}">
   <dimension ref="A1:AB24"/>
   <sheetViews>
@@ -17820,7 +18863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C151C05-E2F4-455A-AEB9-6524417D8442}">
   <dimension ref="A1:AA40"/>
   <sheetViews>
@@ -19204,7 +20247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C91F198-B38A-4DA8-A78C-ABC8E5EDC3C9}">
   <dimension ref="A1:AE15"/>
   <sheetViews>
@@ -19931,7 +20974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8AF431-8396-45B8-B7F5-A36FBD82D208}">
   <dimension ref="A1:V36"/>
   <sheetViews>
@@ -20463,7 +21506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147B5EB0-EC16-485B-8EB9-BF6E6861C707}">
   <dimension ref="A1:V23"/>
   <sheetViews>
@@ -20958,7 +22001,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFCB1861-4C9E-41AD-B401-5FCF8E78F9CE}">
   <dimension ref="A1:AE24"/>
   <sheetViews>
@@ -22169,7 +23212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D435D0C8-2A67-4DFF-8E91-310A628ECB70}">
   <dimension ref="A1:B211"/>
   <sheetViews>
@@ -28739,995 +29782,447 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28AB0DF-12AC-414D-A33D-AB09F26711FA}">
-  <dimension ref="A1:V25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5D6153-C552-49F4-A600-7B60A2A6EEB8}">
+  <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="39.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="23.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="27.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="31.140625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="31" style="1" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23.140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="21.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="18.5703125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="20" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="12.28515625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11" style="1" customWidth="1"/>
-    <col min="29" max="29" width="14.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13.28515625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5703125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="15" style="1" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="15" style="1" customWidth="1"/>
-    <col min="35" max="35" width="15.42578125" style="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="38.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" style="1" customWidth="1"/>
+    <col min="26" max="27" width="15" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15" style="1" customWidth="1"/>
+    <col min="30" max="30" width="15.42578125" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>604</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>797</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>623</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>624</v>
+        <v>17</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>796</v>
+        <v>1541</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>611</v>
+        <v>1542</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>612</v>
+        <v>19</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>613</v>
+        <v>20</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>615</v>
+        <v>21</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>616</v>
+        <v>22</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>1547</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>712</v>
+        <v>1543</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>605</v>
+        <v>422</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="E2" t="s">
-        <v>787</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>715</v>
+        <v>51</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="M2" s="1">
+        <v>15044466025</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1545</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>413</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W2" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>1548</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>1549</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>716</v>
+        <v>1552</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>605</v>
+        <v>482</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="E3" t="s">
-        <v>788</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>720</v>
+        <v>1553</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>605</v>
+        <v>422</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="E4" t="s">
-        <v>789</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>723</v>
+        <v>1554</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>724</v>
+        <v>422</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>725</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="E5" t="s">
-        <v>790</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>795</v>
+        <v>51</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>423</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>804</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="N5"/>
       <c r="Q5" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="E6" t="s">
-        <v>791</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>626</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>732</v>
-      </c>
-      <c r="E7" t="s">
-        <v>792</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>799</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="E8" t="s">
-        <v>793</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>420</v>
-      </c>
-      <c r="E9" t="s">
-        <v>794</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>801</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="E10" t="s">
-        <v>742</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V10" s="1">
-        <v>35801</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>744</v>
-      </c>
-      <c r="E11" t="s">
-        <v>745</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="E12" t="s">
-        <v>748</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="E13" t="s">
-        <v>751</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="E14" t="s">
-        <v>754</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E15" t="s">
-        <v>756</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>757</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="E16" t="s">
-        <v>760</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>733</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="T16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="E17" t="s">
-        <v>763</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>733</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V17" s="1">
-        <v>35801</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>765</v>
-      </c>
-      <c r="E18" t="s">
-        <v>766</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>733</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V18" s="1">
-        <v>35801</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>767</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="E19" t="s">
-        <v>769</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>804</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>770</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="E20" t="s">
-        <v>772</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="E21" t="s">
-        <v>774</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="E22" t="s">
-        <v>777</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>802</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>779</v>
-      </c>
-      <c r="E23" t="s">
-        <v>780</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="E24" t="s">
-        <v>783</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U24" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="E25" t="s">
-        <v>786</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>798</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>117</v>
-      </c>
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N6" s="15"/>
+    </row>
+    <row r="7" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="15"/>
+    </row>
+    <row r="8" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="7:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="7:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="7:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="7:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="N21"/>
+    </row>
+    <row r="22" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="N23"/>
+    </row>
+    <row r="24" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="N24"/>
+    </row>
+    <row r="25" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="N25"/>
+    </row>
+    <row r="26" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="N26"/>
+    </row>
+    <row r="27" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="N27"/>
+    </row>
+    <row r="28" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="N28"/>
+    </row>
+    <row r="29" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="N29"/>
+    </row>
+    <row r="30" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="N30"/>
+    </row>
+    <row r="31" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="N31"/>
+    </row>
+    <row r="32" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="N32"/>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="N33"/>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="N34"/>
+    </row>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="N35"/>
+    </row>
+    <row r="36" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="N36"/>
+    </row>
+    <row r="37" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="N37"/>
+    </row>
+    <row r="38" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>